<commit_message>
fpspreadsheet: Update workbookchartsource demo to show multiple-y-values feature.
git-svn-id: https://svn.code.sf.net/p/lazarus-ccr/svn/components/fpspreadsheet@9046 8e941d3f-bd1b-0410-a28a-d453659cc2b4
</commit_message>
<xml_diff>
--- a/examples/visual/fpschart/workbookchartsource/test-data.xlsx
+++ b/examples/visual/fpschart/workbookchartsource/test-data.xlsx
@@ -1,36 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog_Lazarus\svn\lazarus-ccr\components\fpspreadsheet\examples\visual\fpschart\workbookchartsource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{28B3AEC3-7614-4F7E-B33F-EB2E559673BC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099652E4-363F-4337-921C-C0263B0781B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="330" windowWidth="25170" windowHeight="14955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>cos(x*0.3)</t>
-  </si>
-  <si>
-    <t>sin(x*0.3)</t>
   </si>
   <si>
     <t>Season</t>
@@ -50,14 +47,23 @@
   <si>
     <t>Data</t>
   </si>
+  <si>
+    <t>sin(x)</t>
+  </si>
+  <si>
+    <t>exp(-x/3)</t>
+  </si>
+  <si>
+    <t>exp(-x/3)*sin(3*x)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -96,16 +102,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -124,9 +135,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -164,9 +175,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,26 +210,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,26 +245,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -444,304 +421,563 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="5" width="9.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <f>EXP(-A2/3)*SIN(3*A2)</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <f>SIN(A2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <f>EXP(-A2/3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="B3" s="5">
+        <f t="shared" ref="B3:B32" si="0">EXP(-A3/3)*SIN(3*A3)</f>
+        <v>0.62713793395432627</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C32" si="1">SIN(A3)</f>
+        <v>0.24740395925452294</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D17" si="2">EXP(-A3/3)</f>
+        <v>0.92004441462932329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="B4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84436127683034001</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.47942553860420301</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="2"/>
+        <v>0.84648172489061413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="B5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.60596401502318442</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.68163876002333412</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="2"/>
+        <v>0.77880078307140488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.10111690432332036</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.8414709848078965</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.71653131057378927</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="B7" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.3767964439658994</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.9489846193555862</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="2"/>
+        <v>0.65924063020044377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="B8" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.59290198715637943</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99749498660405445</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.60653065971263342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="B9" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.47931563524622983</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.98398594687393692</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.55803514577004709</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <f>SIN(A2*0.3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <f>SIN(A3*0.3)</f>
-        <v>0.29552020666133955</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3">
-        <f t="shared" ref="B4:B32" si="0">SIN(A4*0.3)</f>
-        <v>0.56464247339503537</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B10" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.14345670009834893</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.90929742682568171</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.51341711903259202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>2.25</v>
+      </c>
+      <c r="B11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.21258576771327323</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.7780731968879212</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.47236655274101469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.40765310948598249</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.59847214410395655</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.4345982085070782</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>2.75</v>
+      </c>
+      <c r="B13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36890297456130111</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.38166099205233167</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.39984965434484737</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.7833269096274833</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.15160991804715873</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14112000805986721</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.36787944117144233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="B15" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.10814619969912632</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.10819513453010837</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.33846542510674221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="B16" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.27394009571918015</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.35078322768961984</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="2"/>
+        <v>0.31140322391459768</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>3.75</v>
+      </c>
+      <c r="B17" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.27728163372663134</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.57156131874234373</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="2"/>
+        <v>0.28650479686019009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.93203908596722629</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B18" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.14143908557531917</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.7568024953079282</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" ref="E18:E32" si="3">EXP(-A18/3)</f>
+        <v>0.26359713811572677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>4.25</v>
+      </c>
+      <c r="B19" s="5">
+        <f t="shared" si="0"/>
+        <v>4.4284138358282113E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.8949893582285835</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24252107463564868</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="B20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.17934854782127702</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.97753011766509701</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="3"/>
+        <v>0.22313016014842982</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>4.75</v>
+      </c>
+      <c r="B21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.20398424140886884</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.99929278897537799</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.20528965757990927</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.99749498660405445</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.12282350782761149</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.95892427466313845</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.18887560283756183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>5.25</v>
+      </c>
+      <c r="B23" s="5">
+        <f t="shared" si="0"/>
+        <v>-7.3027374929054006E-3</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.85893449342659201</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="3"/>
+        <v>0.17377394345044514</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="B24" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.11380005980122339</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.70554032557039192</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15987974607969391</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>5.75</v>
+      </c>
+      <c r="B25" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.14703563879075182</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.50827907749925838</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1470964673929768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.97384763087819526</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B26" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.10163507174892873</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.27941549819892586</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1353352832366127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>6.25</v>
+      </c>
+      <c r="B27" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.2375685928123839E-2</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.3179216547556817E-2</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12451447144412296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="B28" s="5">
+        <f t="shared" si="0"/>
+        <v>6.9369947466560236E-2</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21511998808781552</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="3"/>
+        <v>0.11455884399268773</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>6.75</v>
+      </c>
+      <c r="B29" s="5">
+        <f t="shared" si="0"/>
+        <v>0.10387358254520845</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.45004407378061762</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="3"/>
+        <v>0.10539922456186433</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.86320936664887371</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3">
-        <f t="shared" si="0"/>
-        <v>0.67546318055115095</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="0"/>
-        <v>0.42737988023383017</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" si="0"/>
-        <v>0.14112000805986721</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.15774569414324821</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.44252044329485207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.68776615918397377</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.87157577241358819</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.97753011766509701</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.99616460883584068</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.92581468232773245</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.7727644875559877</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.55068554259763758</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.27941549819892586</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6813900484349713E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3">
-        <f t="shared" si="0"/>
-        <v>0.31154136351337786</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3">
-        <f t="shared" si="0"/>
-        <v>0.57843976438819944</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3">
-        <f t="shared" si="0"/>
-        <v>0.79366786384915267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3">
-        <f t="shared" si="0"/>
+      <c r="B30" s="5">
+        <f t="shared" si="0"/>
+        <v>8.1132143693691719E-2</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.65698659871878906</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="3"/>
+        <v>9.6971967864405054E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>7.25</v>
+      </c>
+      <c r="B31" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1306998956380167E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="1"/>
+        <v>0.82308087901150551</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="3"/>
+        <v>8.9218517409260109E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="B32" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.9989719184919496E-2</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="1"/>
         <v>0.9379999767747389</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" s="3">
-        <f t="shared" si="0"/>
-        <v>0.99854334537460498</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" s="3">
-        <f t="shared" si="0"/>
-        <v>0.9698898108450863</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" s="3">
-        <f t="shared" si="0"/>
-        <v>0.85459890808828043</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3">
-        <f t="shared" si="0"/>
-        <v>0.66296923008218334</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" s="3">
-        <f t="shared" si="0"/>
-        <v>0.41211848524175659</v>
+      <c r="E32" s="2">
+        <f t="shared" si="3"/>
+        <v>8.20849986238988E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -765,7 +1001,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <f t="shared" ref="B2:B27" si="0">COS(A2*0.3)</f>
         <v>1</v>
       </c>
@@ -774,7 +1010,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <f t="shared" si="0"/>
         <v>0.95533648912560598</v>
       </c>
@@ -783,7 +1019,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <f t="shared" si="0"/>
         <v>0.82533561490967833</v>
       </c>
@@ -792,7 +1028,7 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>0.6216099682706645</v>
       </c>
@@ -801,7 +1037,7 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>0.36235775447667362</v>
       </c>
@@ -810,7 +1046,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>7.0737201667702906E-2</v>
       </c>
@@ -819,7 +1055,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>-0.22720209469308689</v>
       </c>
@@ -828,7 +1064,7 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>-0.50484610459985757</v>
       </c>
@@ -837,7 +1073,7 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>-0.73739371554124544</v>
       </c>
@@ -846,7 +1082,7 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>-0.90407214201706099</v>
       </c>
@@ -855,7 +1091,7 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>-0.98999249660044542</v>
       </c>
@@ -864,7 +1100,7 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>-0.98747976990886488</v>
       </c>
@@ -873,7 +1109,7 @@
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>-0.89675841633414721</v>
       </c>
@@ -882,7 +1118,7 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>-0.72593230420014021</v>
       </c>
@@ -891,7 +1127,7 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>-0.49026082134069943</v>
       </c>
@@ -900,7 +1136,7 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>-0.2107957994307797</v>
       </c>
@@ -909,7 +1145,7 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>8.7498983439446398E-2</v>
       </c>
@@ -918,7 +1154,7 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>0.37797774271298024</v>
       </c>
@@ -927,7 +1163,7 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>0.63469287594263391</v>
       </c>
@@ -936,7 +1172,7 @@
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>0.83471278483915978</v>
       </c>
@@ -945,7 +1181,7 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>0.96017028665036597</v>
       </c>
@@ -954,7 +1190,7 @@
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>0.9998586363834151</v>
       </c>
@@ -963,7 +1199,7 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>0.9502325919585296</v>
       </c>
@@ -972,7 +1208,7 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>0.81572510012535737</v>
       </c>
@@ -981,7 +1217,7 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>0.60835131453225522</v>
       </c>
@@ -990,7 +1226,7 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>0.34663531783502582</v>
       </c>
@@ -1002,50 +1238,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>